<commit_message>
Added new analyses to the excel file
</commit_message>
<xml_diff>
--- a/8kN/analysis/RPA/Regen Cooling Geometry Calc.xlsx
+++ b/8kN/analysis/RPA/Regen Cooling Geometry Calc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emilio\Documents\PSAS\liquid-propellant-engine\8kN\analysis\RPA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{246DE623-265B-48CF-A9CD-6C6F9C663701}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7A744D-0A60-48C3-890A-89A31C27DC1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FB21CA52-B782-42C1-96A3-5624C0AF0A2E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
   <si>
     <t>General Inputs</t>
   </si>
@@ -157,6 +157,24 @@
   </si>
   <si>
     <t>Channel area</t>
+  </si>
+  <si>
+    <t>Hydraulic Diameter</t>
+  </si>
+  <si>
+    <t>Throat</t>
+  </si>
+  <si>
+    <t>Chamber</t>
+  </si>
+  <si>
+    <t>Exit</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Other Analyses</t>
   </si>
 </sst>
 </file>
@@ -164,7 +182,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -202,7 +220,7 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD3B773B-E951-4846-B280-CB8511E8D727}">
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,9 +549,10 @@
     <col min="8" max="8" width="15.85546875" style="1" customWidth="1"/>
     <col min="12" max="12" width="14.140625" style="1" customWidth="1"/>
     <col min="13" max="13" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -550,8 +569,11 @@
       <c r="O1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="R1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -590,8 +612,11 @@
       <c r="O2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="R2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>33</v>
       </c>
@@ -633,8 +658,18 @@
       <c r="O3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="R3" t="s">
+        <v>46</v>
+      </c>
+      <c r="S3" s="3">
+        <f>4*1000^2*I6/(2*M3+2*M6)</f>
+        <v>1.0660878696231035</v>
+      </c>
+      <c r="T3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
@@ -676,8 +711,18 @@
       <c r="O4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="R4" t="s">
+        <v>45</v>
+      </c>
+      <c r="S4" s="3">
+        <f>4*1000^2*I6/(2*M4+2*M7)</f>
+        <v>0.81420678470754237</v>
+      </c>
+      <c r="T4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -711,8 +756,18 @@
       <c r="O5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="R5" t="s">
+        <v>47</v>
+      </c>
+      <c r="S5" s="3">
+        <f>4*1000^2*I6/(2*M5+2*M8)</f>
+        <v>1.2102109856882077</v>
+      </c>
+      <c r="T5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -746,8 +801,15 @@
       <c r="O6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="R6" t="s">
+        <v>48</v>
+      </c>
+      <c r="S6" s="3">
+        <f>AVERAGE(S3:S5)</f>
+        <v>1.0301685466729511</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -778,7 +840,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="H8" s="1" t="s">
         <v>22</v>
       </c>
@@ -803,7 +865,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="H9" s="1" t="s">
         <v>23</v>
       </c>
@@ -815,7 +877,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="H10" s="1" t="s">
         <v>24</v>
       </c>
@@ -827,7 +889,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="H11" s="1" t="s">
         <v>27</v>
       </c>
@@ -839,7 +901,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="H12" s="1" t="s">
         <v>28</v>
       </c>
@@ -851,7 +913,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="H13" s="1" t="s">
         <v>29</v>
       </c>
@@ -863,7 +925,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="H14" s="1" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Added a little more analysis to the excel sheet
</commit_message>
<xml_diff>
--- a/8kN/analysis/RPA/Regen Cooling Geometry Calc.xlsx
+++ b/8kN/analysis/RPA/Regen Cooling Geometry Calc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emilio\Documents\PSAS\liquid-propellant-engine\8kN\analysis\RPA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7A744D-0A60-48C3-890A-89A31C27DC1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A0A836-741D-4E8F-A79B-6954990674F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FB21CA52-B782-42C1-96A3-5624C0AF0A2E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="54">
   <si>
     <t>General Inputs</t>
   </si>
@@ -175,6 +175,18 @@
   </si>
   <si>
     <t>Other Analyses</t>
+  </si>
+  <si>
+    <t>Top of Channel radius as a function of chamber radius</t>
+  </si>
+  <si>
+    <t>Chamber radius</t>
+  </si>
+  <si>
+    <t>Channel top radius</t>
+  </si>
+  <si>
+    <t>channel height</t>
   </si>
 </sst>
 </file>
@@ -535,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD3B773B-E951-4846-B280-CB8511E8D727}">
-  <dimension ref="A1:T14"/>
+  <dimension ref="A1:W14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,12 +559,14 @@
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" style="1" customWidth="1"/>
     <col min="8" max="8" width="15.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.140625" style="1" customWidth="1"/>
     <col min="13" max="13" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.140625" style="3"/>
+    <col min="21" max="21" width="22.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -572,8 +586,11 @@
       <c r="R1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="U1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -615,8 +632,17 @@
       <c r="R2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="U2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="V2">
+        <v>78.7</v>
+      </c>
+      <c r="W2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>33</v>
       </c>
@@ -650,7 +676,7 @@
       </c>
       <c r="M3" s="4">
         <f>I10*1000</f>
-        <v>0.63080763774095205</v>
+        <v>1.3868961315803312</v>
       </c>
       <c r="N3" t="s">
         <v>7</v>
@@ -663,13 +689,23 @@
       </c>
       <c r="S3" s="3">
         <f>4*1000^2*I6/(2*M3+2*M6)</f>
-        <v>1.0660878696231035</v>
+        <v>2.0882050765745137</v>
       </c>
       <c r="T3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="U3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="V3" s="2">
+        <f>(((2*PI()*V2/1000)-B6*B7)/B7)</f>
+        <v>4.224296485278149E-3</v>
+      </c>
+      <c r="W3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
@@ -693,7 +729,7 @@
       </c>
       <c r="I4" s="2">
         <f>(I3-B6*B7)/B7</f>
-        <v>4.4411279165865945E-4</v>
+        <v>7.2979825693510257E-4</v>
       </c>
       <c r="J4" t="s">
         <v>8</v>
@@ -703,7 +739,7 @@
       </c>
       <c r="M4" s="4">
         <f>I5*1000</f>
-        <v>4.885240708245254</v>
+        <v>8.0277808262861274</v>
       </c>
       <c r="N4" t="s">
         <v>7</v>
@@ -716,13 +752,23 @@
       </c>
       <c r="S4" s="3">
         <f>4*1000^2*I6/(2*M4+2*M7)</f>
-        <v>0.81420678470754237</v>
+        <v>1.337963471047688</v>
       </c>
       <c r="T4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="V4" s="3">
+        <f>(V2/1000+B5+V3)*1000</f>
+        <v>84.194296485278159</v>
+      </c>
+      <c r="W4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -738,7 +784,7 @@
       </c>
       <c r="I5" s="2">
         <f>I4*B2</f>
-        <v>4.885240708245254E-3</v>
+        <v>8.027780826286128E-3</v>
       </c>
       <c r="J5" t="s">
         <v>8</v>
@@ -748,7 +794,7 @@
       </c>
       <c r="M5" s="4">
         <f>I14*1000</f>
-        <v>0.77081816931993075</v>
+        <v>1.6760833368195731</v>
       </c>
       <c r="N5" t="s">
         <v>7</v>
@@ -761,13 +807,13 @@
       </c>
       <c r="S5" s="3">
         <f>4*1000^2*I6/(2*M5+2*M8)</f>
-        <v>1.2102109856882077</v>
+        <v>2.2657357046131708</v>
       </c>
       <c r="T5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -783,7 +829,7 @@
       </c>
       <c r="I6" s="2">
         <f>I4*I5</f>
-        <v>2.1695978888633264E-6</v>
+        <v>5.8586604540806539E-6</v>
       </c>
       <c r="J6" t="s">
         <v>20</v>
@@ -793,7 +839,7 @@
       </c>
       <c r="M6" s="4">
         <f>I9*1000</f>
-        <v>3.4393969873812704</v>
+        <v>4.224296485278149</v>
       </c>
       <c r="N6" t="s">
         <v>7</v>
@@ -806,15 +852,15 @@
       </c>
       <c r="S6" s="3">
         <f>AVERAGE(S3:S5)</f>
-        <v>1.0301685466729511</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+        <v>1.8973014174117908</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B7">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>21</v>
@@ -831,7 +877,7 @@
       </c>
       <c r="M7" s="4">
         <f>I4*1000</f>
-        <v>0.44411279165865947</v>
+        <v>0.72979825693510258</v>
       </c>
       <c r="N7" t="s">
         <v>7</v>
@@ -840,7 +886,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="H8" s="1" t="s">
         <v>22</v>
       </c>
@@ -856,7 +902,7 @@
       </c>
       <c r="M8" s="4">
         <f>I13*1000</f>
-        <v>2.8146688482674143</v>
+        <v>3.4954469896453162</v>
       </c>
       <c r="N8" t="s">
         <v>7</v>
@@ -865,31 +911,31 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="H9" s="1" t="s">
         <v>23</v>
       </c>
       <c r="I9" s="2">
         <f>(I8-B6*B7)/B7</f>
-        <v>3.4393969873812704E-3</v>
+        <v>4.224296485278149E-3</v>
       </c>
       <c r="J9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="H10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="I10" s="2">
         <f>I6/I9</f>
-        <v>6.3080763774095211E-4</v>
+        <v>1.3868961315803311E-3</v>
       </c>
       <c r="J10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="H11" s="1" t="s">
         <v>27</v>
       </c>
@@ -901,7 +947,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="H12" s="1" t="s">
         <v>28</v>
       </c>
@@ -913,25 +959,25 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="H13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="I13" s="2">
         <f>(I12-B6*B7)/B7</f>
-        <v>2.8146688482674144E-3</v>
+        <v>3.4954469896453164E-3</v>
       </c>
       <c r="J13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="H14" s="1" t="s">
         <v>30</v>
       </c>
       <c r="I14" s="2">
         <f>I6/I13</f>
-        <v>7.7081816931993073E-4</v>
+        <v>1.6760833368195732E-3</v>
       </c>
       <c r="J14" t="s">
         <v>8</v>

</xml_diff>